<commit_message>
Add latest 816 data and standard offer data
</commit_message>
<xml_diff>
--- a/retail-power-compare/raw/monthly_standard_offer_by_utility.xlsx
+++ b/retail-power-compare/raw/monthly_standard_offer_by_utility.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Darren/Github clones/data-projects/retail-power-compare/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C151948-DE52-B542-B749-7EEC0518D562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BE529E-1627-8947-846E-7C62BA337ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20100" windowHeight="27020" xr2:uid="{CAE620D4-FD76-9349-A05C-D8713AA01DE9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="8">
   <si>
     <t>Utility</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C04127-8BFC-3147-AA20-C61BC9431E16}">
-  <dimension ref="A1:D361"/>
+  <dimension ref="A1:D397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D357" sqref="D357"/>
+    <sheetView tabSelected="1" topLeftCell="A374" workbookViewId="0">
+      <selection activeCell="C400" sqref="C400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5120,6 +5120,474 @@
         <v>6.0267000000000001E-2</v>
       </c>
     </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A362" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B362" t="s">
+        <v>7</v>
+      </c>
+      <c r="C362" t="s">
+        <v>5</v>
+      </c>
+      <c r="D362" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A363" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B363" t="s">
+        <v>7</v>
+      </c>
+      <c r="C363" t="s">
+        <v>5</v>
+      </c>
+      <c r="D363" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A364" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B364" t="s">
+        <v>7</v>
+      </c>
+      <c r="C364" t="s">
+        <v>5</v>
+      </c>
+      <c r="D364" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A365" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B365" t="s">
+        <v>7</v>
+      </c>
+      <c r="C365" t="s">
+        <v>5</v>
+      </c>
+      <c r="D365" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A366" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B366" t="s">
+        <v>7</v>
+      </c>
+      <c r="C366" t="s">
+        <v>5</v>
+      </c>
+      <c r="D366" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A367" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B367" t="s">
+        <v>7</v>
+      </c>
+      <c r="C367" t="s">
+        <v>5</v>
+      </c>
+      <c r="D367" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A368" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B368" t="s">
+        <v>7</v>
+      </c>
+      <c r="C368" t="s">
+        <v>5</v>
+      </c>
+      <c r="D368" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A369" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B369" t="s">
+        <v>7</v>
+      </c>
+      <c r="C369" t="s">
+        <v>5</v>
+      </c>
+      <c r="D369" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A370" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B370" t="s">
+        <v>7</v>
+      </c>
+      <c r="C370" t="s">
+        <v>5</v>
+      </c>
+      <c r="D370" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A371" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B371" t="s">
+        <v>7</v>
+      </c>
+      <c r="C371" t="s">
+        <v>5</v>
+      </c>
+      <c r="D371" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A372" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B372" t="s">
+        <v>7</v>
+      </c>
+      <c r="C372" t="s">
+        <v>5</v>
+      </c>
+      <c r="D372" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A373" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B373" t="s">
+        <v>7</v>
+      </c>
+      <c r="C373" t="s">
+        <v>5</v>
+      </c>
+      <c r="D373" s="2">
+        <v>0.110873</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A374" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B374" t="s">
+        <v>7</v>
+      </c>
+      <c r="C374" t="s">
+        <v>4</v>
+      </c>
+      <c r="D374" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A375" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B375" t="s">
+        <v>7</v>
+      </c>
+      <c r="C375" t="s">
+        <v>4</v>
+      </c>
+      <c r="D375" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A376" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B376" t="s">
+        <v>7</v>
+      </c>
+      <c r="C376" t="s">
+        <v>4</v>
+      </c>
+      <c r="D376" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A377" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B377" t="s">
+        <v>7</v>
+      </c>
+      <c r="C377" t="s">
+        <v>4</v>
+      </c>
+      <c r="D377" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A378" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B378" t="s">
+        <v>7</v>
+      </c>
+      <c r="C378" t="s">
+        <v>4</v>
+      </c>
+      <c r="D378" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A379" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B379" t="s">
+        <v>7</v>
+      </c>
+      <c r="C379" t="s">
+        <v>4</v>
+      </c>
+      <c r="D379" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A380" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B380" t="s">
+        <v>7</v>
+      </c>
+      <c r="C380" t="s">
+        <v>4</v>
+      </c>
+      <c r="D380" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A381" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B381" t="s">
+        <v>7</v>
+      </c>
+      <c r="C381" t="s">
+        <v>4</v>
+      </c>
+      <c r="D381" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A382" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B382" t="s">
+        <v>7</v>
+      </c>
+      <c r="C382" t="s">
+        <v>4</v>
+      </c>
+      <c r="D382" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A383" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B383" t="s">
+        <v>7</v>
+      </c>
+      <c r="C383" t="s">
+        <v>4</v>
+      </c>
+      <c r="D383" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A384" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B384" t="s">
+        <v>7</v>
+      </c>
+      <c r="C384" t="s">
+        <v>4</v>
+      </c>
+      <c r="D384" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A385" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B385" t="s">
+        <v>7</v>
+      </c>
+      <c r="C385" t="s">
+        <v>4</v>
+      </c>
+      <c r="D385" s="2">
+        <v>0.11684</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A386" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B386" t="s">
+        <v>3</v>
+      </c>
+      <c r="D386" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A387" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B387" t="s">
+        <v>3</v>
+      </c>
+      <c r="D387" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A388" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B388" t="s">
+        <v>3</v>
+      </c>
+      <c r="D388" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A389" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B389" t="s">
+        <v>3</v>
+      </c>
+      <c r="D389" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A390" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B390" t="s">
+        <v>3</v>
+      </c>
+      <c r="D390" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A391" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B391" t="s">
+        <v>3</v>
+      </c>
+      <c r="D391" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A392" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B392" t="s">
+        <v>3</v>
+      </c>
+      <c r="D392" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A393" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B393" t="s">
+        <v>3</v>
+      </c>
+      <c r="D393" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A394" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B394" t="s">
+        <v>3</v>
+      </c>
+      <c r="D394" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A395" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B395" t="s">
+        <v>3</v>
+      </c>
+      <c r="D395" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A396" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B396" t="s">
+        <v>3</v>
+      </c>
+      <c r="D396" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A397" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B397" t="s">
+        <v>3</v>
+      </c>
+      <c r="D397" s="2">
+        <v>0.118161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>